<commit_message>
added source filed for MRLF. updated publisher mapping
</commit_message>
<xml_diff>
--- a/landlibrary/importers/Mekong Land Research Forum/publishers-mapping (MLRF-LP).xlsx
+++ b/landlibrary/importers/Mekong Land Research Forum/publishers-mapping (MLRF-LP).xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lisette/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\data\landlibrary\importers\Mekong Land Research Forum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14484"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>Elsevier Ltd</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Land Deal Politics Initiative (LDPI)</t>
   </si>
   <si>
-    <t>DO NOT ENTER - NO WAY TO TELL WHICH ORGANIZATION</t>
-  </si>
-  <si>
     <t>NUS Press Singapore</t>
   </si>
   <si>
@@ -198,12 +195,30 @@
   </si>
   <si>
     <t>International Federation of Surveyors (FIG)</t>
+  </si>
+  <si>
+    <t>Blackwell Publishing Asia</t>
+  </si>
+  <si>
+    <t>Cornell University Press</t>
+  </si>
+  <si>
+    <t>International Organization on Migration (IOM) and the Asia Research Center on Migration (ARCM), Institute of Asian Studies, Chulalongkorn University.</t>
+  </si>
+  <si>
+    <t>NUS Press</t>
+  </si>
+  <si>
+    <t>Save Cambodia's Wildlife</t>
+  </si>
+  <si>
+    <t>International Organization for Migration; Asian Research Center for Migration; Chulalongkorn University</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,6 +239,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -259,7 +275,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,19 +554,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="77.1640625" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="119.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -558,7 +574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -566,7 +582,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -574,7 +590,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -582,7 +598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -590,7 +606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -598,227 +614,259 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>19</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added source fiel for MLRF importer. updated publisher for MLRF2
</commit_message>
<xml_diff>
--- a/landlibrary/importers/Mekong Land Research Forum/publishers-mapping (MLRF-LP).xlsx
+++ b/landlibrary/importers/Mekong Land Research Forum/publishers-mapping (MLRF-LP).xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>Elsevier Ltd</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>International Organization for Migration; Asian Research Center for Migration; Chulalongkorn University</t>
+  </si>
+  <si>
+    <t>BRICS Initiatives for Critical Agrarian Studies (BICAS), MOSAIC Research Project, Land Deal Politics Initiative (LDPI), RCSD Chiang Mai University, Transnational Institute</t>
+  </si>
+  <si>
+    <t>BRICS Initiatives in Critical Agrarian Studies;International Institute of Social Studies;Land Deal Politics Initiative;Regional Center for Social Science and Sustainable Development - Chiang Mai University;Transnational Institute</t>
   </si>
 </sst>
 </file>
@@ -542,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,6 +848,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:A46">
     <sortCondition ref="A1"/>

</xml_diff>